<commit_message>
adds missing data in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/adult-juvenile-steelhead-data-metadata.xlsx
+++ b/data-raw/metadata/adult-juvenile-steelhead-data-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EKeller\Desktop\Steelhead EDI\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB60A85-04E6-492A-B95D-A9B4C7BAA0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF0ECB4-1991-A148-9F37-C13585E143DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="40" windowWidth="13880" windowHeight="10200" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -167,24 +167,32 @@
   </si>
   <si>
     <t>whole</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>2021-02-02</t>
+  </si>
+  <si>
+    <t>2022-04-27</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>steelhead</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -221,12 +229,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -234,10 +241,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,313 +629,498 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="1"/>
-    <col min="2" max="2" width="38.9140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="4" customWidth="1"/>
     <col min="14" max="1021" width="19.6640625" style="1"/>
     <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="F6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="5" t="s">
+      <c r="F7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="I7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="5" t="s">
+      <c r="F8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="C9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="F9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="C10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5" t="s">
+      <c r="F10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="5" t="s">
+      <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="I11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="C12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="5" t="s">
+      <c r="F12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="C13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="C14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="5" t="s">
+      <c r="F14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>46</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -962,25 +1154,25 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
updates metadata to reflect new columsn in steelhead csv
</commit_message>
<xml_diff>
--- a/data-raw/metadata/adult-juvenile-steelhead-data-metadata.xlsx
+++ b/data-raw/metadata/adult-juvenile-steelhead-data-metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/stanislaus-steelhead/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF0ECB4-1991-A148-9F37-C13585E143DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40738D37-AA2D-FF47-8332-A690EBD85DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="61">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -182,6 +182,33 @@
   </si>
   <si>
     <t>steelhead</t>
+  </si>
+  <si>
+    <t>survey_week</t>
+  </si>
+  <si>
+    <t>Week of the year that sampling occurred</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>survey_year</t>
+  </si>
+  <si>
+    <t>Year sampling occurred</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>was_surveyed</t>
+  </si>
+  <si>
+    <t>Whether or not sampling occurred during that week, riffle, and year.</t>
+  </si>
+  <si>
+    <t>ordinal</t>
   </si>
 </sst>
 </file>
@@ -229,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,10 +268,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG14"/>
+  <dimension ref="A1:AMG17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,488 +678,583 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="5"/>
+      <c r="L2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="7">
+        <v>2021</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C6" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C7" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="F8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7">
+      <c r="I8" s="5"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3">
         <v>0</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M8" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="7">
+      <c r="I9" s="5"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3">
         <v>0</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M9" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7">
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3">
         <v>0</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7">
+      <c r="I11" s="5"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3">
         <v>0</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M11" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="7">
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M12" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="7">
+      <c r="I13" s="5"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M13" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7">
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3">
         <v>0</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M14" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="7">
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3">
         <v>0</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M15" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7">
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="3">
         <v>0</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M16" s="3">
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="7">
+      <c r="I17" s="5"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="3">
         <v>0</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M17" s="3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1021" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1024" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1021" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1024" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1021" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1024" xr:uid="{00000000-0002-0000-0800-000003000000}">
       <formula1>"ratio,interval"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>